<commit_message>
updated on June 19
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\eclipse-workspace\MakeMyTripBusBooking\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72944D0A-25ED-416B-BD3D-43D2E688C61A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C098A01-45F8-4AE8-A0CA-F30A479A49CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="2" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +481,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="6">
-        <v>45826</v>
+        <v>45836</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>

</xml_diff>